<commit_message>
fix: Update login_data.xlsx with new test data
</commit_message>
<xml_diff>
--- a/test_data/login_data.xlsx
+++ b/test_data/login_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anike\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varun\OneDrive\Desktop\GE\WEB AUTOMATION\orange_hrm\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F088B3B4-633A-4509-8DC7-9839975975BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05515059-29EF-4060-A2C9-7DB8485C2372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C7CFF12F-DAF7-4A6B-994A-77BC86A31C58}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{C7CFF12F-DAF7-4A6B-994A-77BC86A31C58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,12 +51,6 @@
     <t>admin123</t>
   </si>
   <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>fail</t>
-  </si>
-  <si>
     <t>admin@123</t>
   </si>
   <si>
@@ -64,6 +58,12 @@
   </si>
   <si>
     <t>adm</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,18 +467,18 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -486,10 +486,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -497,10 +497,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>